<commit_message>
revision prepare for hpc analysis
</commit_message>
<xml_diff>
--- a/paper/List_drugs_CCLE.xlsx
+++ b/paper/List_drugs_CCLE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastien.delandtshe\Dropbox\Main\Py\deep_onco_ai\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastien.delandtshe\PycharmProjects\DeepOncoAI\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43F9BAC-DF02-4325-9066-F271367527F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCLE_NP24.2009_profiling_2012.0" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="115">
   <si>
     <t>Compound (code or generic name)</t>
   </si>
@@ -358,12 +359,18 @@
   </si>
   <si>
     <t>Launched-1996</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,7 +507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -683,6 +690,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,9 +860,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1170,21 +1184,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" activeCellId="5" sqref="A13:XFD13 A9:XFD9 A6:XFD6 A16:XFD16 A14:XFD14 A23:XFD23"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1207,8 +1221,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -1229,9 +1243,12 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="J2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
@@ -1252,8 +1269,11 @@
       <c r="G3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1273,7 +1293,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1296,7 +1316,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1316,7 +1336,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1339,7 +1359,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1362,7 +1382,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1385,7 +1405,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1408,7 +1428,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1431,7 +1451,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1451,7 +1471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -1471,7 +1491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -1491,7 +1511,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1511,8 +1531,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1530,9 +1550,12 @@
       <c r="G16" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="J16" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B17" t="s">
@@ -1553,8 +1576,11 @@
       <c r="G17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -1574,7 +1600,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -1594,7 +1620,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -1617,7 +1643,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1637,8 +1663,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B22" t="s">
@@ -1659,9 +1685,12 @@
       <c r="G22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="J22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1682,9 +1711,12 @@
       <c r="G23" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="J23" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B24" t="s">
@@ -1705,8 +1737,11 @@
       <c r="G24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>110</v>
       </c>

</xml_diff>